<commit_message>
step 2 is now complete
</commit_message>
<xml_diff>
--- a/bot_outputs/step_2_out.xlsx
+++ b/bot_outputs/step_2_out.xlsx
@@ -71,6 +71,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="00FFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00EE1111"/>
+          <bgColor rgb="00EE1111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -12948,6 +12962,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" priority="1" dxfId="0" stopIfTrue="0">
+      <formula>=OR(AND(SUM(E2:E4)&lt;&gt;1, SUM(E2:E4)&gt;0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>